<commit_message>
complete refact according excel and reduce method
</commit_message>
<xml_diff>
--- a/DienmayXANH-TestData.xlsx
+++ b/DienmayXANH-TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\eclipse-workspace\DienmayXANH\DienMayXanh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA12EAB1-50B8-4B0B-A57C-457FBA5E7AA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410D22F8-916E-4428-84C1-493350E76E9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ChooseReceivedPlace" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="188">
   <si>
     <t>Inputs</t>
   </si>
@@ -597,6 +597,9 @@
   </si>
   <si>
     <t>ALERT</t>
+  </si>
+  <si>
+    <t>SORTING</t>
   </si>
   <si>
     <t>PASSED</t>
@@ -1104,7 +1107,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1212,6 +1215,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1782,12 +1791,12 @@
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
-      <c r="F1" s="49" t="s">
+      <c r="F1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
       <c r="J1" s="11"/>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.35">
@@ -1939,16 +1948,16 @@
       <c r="J6" s="11"/>
     </row>
     <row r="7" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="50" t="s">
+      <c r="A7" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="45" t="s">
+      <c r="D7" s="47" t="s">
         <v>31</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -1969,10 +1978,10 @@
       <c r="J7" s="11"/>
     </row>
     <row r="8" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="40"/>
-      <c r="B8" s="50"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="46"/>
+      <c r="A8" s="42"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="48"/>
       <c r="E8" s="4" t="s">
         <v>12</v>
       </c>
@@ -1991,16 +2000,16 @@
       <c r="J8" s="11"/>
     </row>
     <row r="9" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="41" t="s">
+      <c r="A9" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="45" t="s">
+      <c r="D9" s="47" t="s">
         <v>39</v>
       </c>
       <c r="E9" s="4" t="s">
@@ -2021,10 +2030,10 @@
       <c r="J9" s="11"/>
     </row>
     <row r="10" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="40"/>
-      <c r="B10" s="42"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="46"/>
+      <c r="A10" s="42"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="48"/>
       <c r="E10" s="4" t="s">
         <v>12</v>
       </c>
@@ -2043,16 +2052,16 @@
       <c r="J10" s="11"/>
     </row>
     <row r="11" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="47" t="s">
+      <c r="A11" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="45" t="s">
+      <c r="D11" s="47" t="s">
         <v>45</v>
       </c>
       <c r="E11" s="4" t="s">
@@ -2073,10 +2082,10 @@
       <c r="J11" s="11"/>
     </row>
     <row r="12" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="40"/>
-      <c r="B12" s="42"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="46"/>
+      <c r="A12" s="42"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="48"/>
       <c r="E12" s="4" t="s">
         <v>12</v>
       </c>
@@ -2178,10 +2187,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="52"/>
+      <c r="G1" s="54"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -2563,13 +2572,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -2902,8 +2911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B3FA518-8AB1-49EC-8FDF-D7AA948B07E0}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2921,12 +2930,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="55" t="s">
+      <c r="F1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
       <c r="J1" s="38"/>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2975,7 +2984,7 @@
         <v>133</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5" t="s">
@@ -3005,7 +3014,7 @@
         <v>133</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>135</v>
@@ -3037,7 +3046,7 @@
         <v>138</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>137</v>
@@ -3067,7 +3076,7 @@
         <v>138</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>137</v>
@@ -3099,7 +3108,7 @@
         <v>143</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>142</v>
@@ -3156,10 +3165,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86148902-2347-4FB2-AC60-64E22A6D30AB}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3170,18 +3179,19 @@
     <col min="4" max="4" customWidth="true" style="1" width="28.33203125" collapsed="true"/>
     <col min="5" max="5" customWidth="true" style="1" width="12.88671875" collapsed="true"/>
     <col min="6" max="6" customWidth="true" style="1" width="15.33203125" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" style="1" width="15.0" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="8.88671875" collapsed="true"/>
+    <col min="7" max="9" customWidth="true" style="1" width="15.0" collapsed="true"/>
+    <col min="10" max="16384" style="1" width="8.88671875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="57" t="s">
+    <row r="1" spans="1:9" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-    </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="40"/>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -3206,8 +3216,11 @@
       <c r="H2" s="3" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="37" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -3228,8 +3241,9 @@
         <v>149</v>
       </c>
       <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I3" s="39"/>
+    </row>
+    <row r="4" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
@@ -3250,8 +3264,9 @@
         <v>149</v>
       </c>
       <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I4" s="39"/>
+    </row>
+    <row r="5" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -3264,7 +3279,9 @@
       <c r="D5" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>187</v>
+      </c>
       <c r="F5" s="4" t="s">
         <v>148</v>
       </c>
@@ -3274,8 +3291,11 @@
       <c r="H5" s="4" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I5" s="39" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
@@ -3288,7 +3308,9 @@
       <c r="D6" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="E6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>187</v>
+      </c>
       <c r="F6" s="4" t="s">
         <v>148</v>
       </c>
@@ -3298,8 +3320,11 @@
       <c r="H6" s="4" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I6" s="39" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -3312,16 +3337,17 @@
       <c r="D7" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>187</v>
+      </c>
       <c r="F7" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>149</v>
-      </c>
+      <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="39"/>
+    </row>
+    <row r="8" spans="1:9" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
         <v>161</v>
       </c>
@@ -3375,11 +3401,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="58" t="s">
+      <c r="F1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">

</xml_diff>

<commit_message>
apply page object model for choose received place
</commit_message>
<xml_diff>
--- a/DienmayXANH-TestData.xlsx
+++ b/DienmayXANH-TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3rdyears\autotestpractice\project\dienmayXANH\github\DienMayXanh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEE37E3-F96F-4584-B974-B0EAA2D379DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB87F84-2F4B-4A68-89B1-B9DEE2CFF1EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="186">
   <si>
     <t>Inputs</t>
   </si>
@@ -587,16 +587,16 @@
     <t>https://www.bachhoaxanh.com/</t>
   </si>
   <si>
+    <t>testSuccessWithOnlyProvince</t>
+  </si>
+  <si>
+    <t>Bình Định</t>
+  </si>
+  <si>
+    <t>FAILED</t>
+  </si>
+  <si>
     <t>PASSED</t>
-  </si>
-  <si>
-    <t>testSuccessWithOnlyProvince</t>
-  </si>
-  <si>
-    <t>FAILED</t>
-  </si>
-  <si>
-    <t>Bình Định</t>
   </si>
 </sst>
 </file>
@@ -1253,56 +1253,56 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1812,7 +1812,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="E11" sqref="E11:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1833,12 +1833,12 @@
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
       <c r="J1" s="11"/>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.35">
@@ -1885,7 +1885,7 @@
         <v>16</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F3" s="25" t="s">
         <v>12</v>
@@ -1906,7 +1906,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>11</v>
@@ -1915,7 +1915,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F4" s="24" t="s">
         <v>18</v>
@@ -1945,7 +1945,7 @@
         <v>23</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F5" s="24" t="s">
         <v>20</v>
@@ -1975,10 +1975,10 @@
         <v>27</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="F6" s="31" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G6" s="24" t="s">
         <v>26</v>
@@ -1992,20 +1992,20 @@
       <c r="J6" s="11"/>
     </row>
     <row r="7" spans="1:10" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="40" t="s">
+      <c r="A7" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="43" t="s">
+      <c r="D7" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="45" t="s">
-        <v>182</v>
+      <c r="E7" s="52" t="s">
+        <v>185</v>
       </c>
       <c r="F7" s="28" t="s">
         <v>29</v>
@@ -2022,11 +2022,11 @@
       <c r="J7" s="11"/>
     </row>
     <row r="8" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="39"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="46"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="53"/>
       <c r="F8" s="26" t="s">
         <v>12</v>
       </c>
@@ -2042,20 +2042,20 @@
       <c r="J8" s="11"/>
     </row>
     <row r="9" spans="1:10" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="49" t="s">
+      <c r="A9" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="43" t="s">
+      <c r="D9" s="45" t="s">
         <v>38</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F9" s="29" t="s">
         <v>34</v>
@@ -2072,10 +2072,10 @@
       <c r="J9" s="11"/>
     </row>
     <row r="10" spans="1:10" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="39"/>
-      <c r="B10" s="50"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="44"/>
+      <c r="A10" s="40"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="46"/>
       <c r="E10" s="4" t="s">
         <v>12</v>
       </c>
@@ -2094,20 +2094,20 @@
       <c r="J10" s="11"/>
     </row>
     <row r="11" spans="1:10" ht="26" x14ac:dyDescent="0.35">
-      <c r="A11" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="53" t="s">
+      <c r="A11" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="41" t="s">
+      <c r="C11" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="43" t="s">
+      <c r="D11" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="47" t="s">
-        <v>182</v>
+      <c r="E11" s="37" t="s">
+        <v>185</v>
       </c>
       <c r="F11" s="24" t="s">
         <v>40</v>
@@ -2124,11 +2124,11 @@
       <c r="J11" s="11"/>
     </row>
     <row r="12" spans="1:10" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="39"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="48"/>
+      <c r="A12" s="40"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="38"/>
       <c r="F12" s="24" t="s">
         <v>44</v>
       </c>
@@ -2169,6 +2169,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
@@ -2178,12 +2184,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:E7 E9:E11">
     <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
@@ -3377,7 +3377,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3439,9 +3439,7 @@
       <c r="D3" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>182</v>
-      </c>
+      <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
         <v>147</v>
       </c>
@@ -3646,15 +3644,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007916DAE6CBAB0E478E10A9FCA3CC0E19" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cc4eab9cdd79106b7ff0c84dd396c527">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="73b10483-4eab-47d9-97c6-997f49bd58aa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9c952eea70f5f85d64c583e57f778f77" ns2:_="">
     <xsd:import namespace="73b10483-4eab-47d9-97c6-997f49bd58aa"/>
@@ -3818,6 +3807,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -3825,14 +3823,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDA4E934-81D4-4CDA-A90D-B17985E7C5D3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF365504-DE0C-4D20-AADF-110855E1E7ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3850,6 +3840,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDA4E934-81D4-4CDA-A90D-B17985E7C5D3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D94FA3B0-7E84-4ED3-9FBD-9B6763F81478}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
complete POM for Comment and ViewListProducts
</commit_message>
<xml_diff>
--- a/DienmayXANH-TestData.xlsx
+++ b/DienmayXANH-TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\eclipse-workspace\DienmayXANH\DienMayXanh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410D22F8-916E-4428-84C1-493350E76E9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84EACD59-5281-4D2E-86F4-6FE4C4B22175}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -713,7 +713,7 @@
       <name val="Trebuchet MS"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -748,6 +748,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF002060"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1220,8 +1226,11 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1229,6 +1238,21 @@
     <xf numFmtId="0" fontId="13" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1241,25 +1265,7 @@
     <xf numFmtId="0" fontId="13" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1791,12 +1797,12 @@
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
       <c r="J1" s="11"/>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.35">
@@ -1948,13 +1954,13 @@
       <c r="J6" s="11"/>
     </row>
     <row r="7" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="52" t="s">
+      <c r="A7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="50" t="s">
+      <c r="C7" s="45" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="47" t="s">
@@ -1978,9 +1984,9 @@
       <c r="J7" s="11"/>
     </row>
     <row r="8" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="42"/>
-      <c r="B8" s="52"/>
-      <c r="C8" s="53"/>
+      <c r="A8" s="43"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="46"/>
       <c r="D8" s="48"/>
       <c r="E8" s="4" t="s">
         <v>12</v>
@@ -2000,13 +2006,13 @@
       <c r="J8" s="11"/>
     </row>
     <row r="9" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="43" t="s">
+      <c r="A9" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="51" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="47" t="s">
@@ -2030,9 +2036,9 @@
       <c r="J9" s="11"/>
     </row>
     <row r="10" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="42"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="46"/>
+      <c r="A10" s="43"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="52"/>
       <c r="D10" s="48"/>
       <c r="E10" s="4" t="s">
         <v>12</v>
@@ -2052,13 +2058,13 @@
       <c r="J10" s="11"/>
     </row>
     <row r="11" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="49" t="s">
+      <c r="A11" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="50" t="s">
+      <c r="C11" s="45" t="s">
         <v>11</v>
       </c>
       <c r="D11" s="47" t="s">
@@ -2082,9 +2088,9 @@
       <c r="J11" s="11"/>
     </row>
     <row r="12" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="42"/>
-      <c r="B12" s="44"/>
-      <c r="C12" s="46"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="52"/>
       <c r="D12" s="48"/>
       <c r="E12" s="4" t="s">
         <v>12</v>
@@ -2129,11 +2135,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="C9:C10"/>
@@ -2142,6 +2143,11 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:E12">
     <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
@@ -2912,7 +2918,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E7"/>
+      <selection activeCell="E9" sqref="E3:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3168,7 +3174,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:E7"/>
+      <selection activeCell="E7" sqref="E5:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3651,6 +3657,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007916DAE6CBAB0E478E10A9FCA3CC0E19" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cc4eab9cdd79106b7ff0c84dd396c527">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="73b10483-4eab-47d9-97c6-997f49bd58aa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9c952eea70f5f85d64c583e57f778f77" ns2:_="">
     <xsd:import namespace="73b10483-4eab-47d9-97c6-997f49bd58aa"/>
@@ -3814,15 +3829,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -3830,6 +3836,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDA4E934-81D4-4CDA-A90D-B17985E7C5D3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF365504-DE0C-4D20-AADF-110855E1E7ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3847,14 +3861,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDA4E934-81D4-4CDA-A90D-B17985E7C5D3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D94FA3B0-7E84-4ED3-9FBD-9B6763F81478}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
done pom for choose received place and view product through list class
</commit_message>
<xml_diff>
--- a/DienmayXANH-TestData.xlsx
+++ b/DienmayXANH-TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3rdyears\autotestpractice\project\dienmayXANH\github\DienMayXanh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB87F84-2F4B-4A68-89B1-B9DEE2CFF1EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADAC3FF1-A6B6-481D-9F61-1AA5C09EFE7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ChooseReceivedPlace" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="185">
   <si>
     <t>Inputs</t>
   </si>
@@ -591,9 +591,6 @@
   </si>
   <si>
     <t>Bình Định</t>
-  </si>
-  <si>
-    <t>FAILED</t>
   </si>
   <si>
     <t>PASSED</t>
@@ -1253,18 +1250,42 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1277,32 +1298,8 @@
     <xf numFmtId="0" fontId="13" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1811,8 +1808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1833,12 +1830,12 @@
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
-      <c r="F1" s="49" t="s">
+      <c r="F1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
       <c r="J1" s="11"/>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.35">
@@ -1885,7 +1882,7 @@
         <v>16</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F3" s="25" t="s">
         <v>12</v>
@@ -1915,7 +1912,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F4" s="24" t="s">
         <v>18</v>
@@ -1945,7 +1942,7 @@
         <v>23</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F5" s="24" t="s">
         <v>20</v>
@@ -1992,20 +1989,20 @@
       <c r="J6" s="11"/>
     </row>
     <row r="7" spans="1:10" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="50" t="s">
+      <c r="A7" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="45" t="s">
+      <c r="D7" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="52" t="s">
-        <v>185</v>
+      <c r="E7" s="45" t="s">
+        <v>184</v>
       </c>
       <c r="F7" s="28" t="s">
         <v>29</v>
@@ -2022,11 +2019,11 @@
       <c r="J7" s="11"/>
     </row>
     <row r="8" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="40"/>
-      <c r="B8" s="50"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="53"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="46"/>
       <c r="F8" s="26" t="s">
         <v>12</v>
       </c>
@@ -2042,20 +2039,20 @@
       <c r="J8" s="11"/>
     </row>
     <row r="9" spans="1:10" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="41" t="s">
+      <c r="A9" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="45" t="s">
+      <c r="D9" s="43" t="s">
         <v>38</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F9" s="29" t="s">
         <v>34</v>
@@ -2072,13 +2069,11 @@
       <c r="J9" s="11"/>
     </row>
     <row r="10" spans="1:10" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="40"/>
-      <c r="B10" s="42"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="A10" s="39"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="4"/>
       <c r="F10" s="32" t="s">
         <v>12</v>
       </c>
@@ -2094,20 +2089,20 @@
       <c r="J10" s="11"/>
     </row>
     <row r="11" spans="1:10" ht="26" x14ac:dyDescent="0.35">
-      <c r="A11" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="47" t="s">
+      <c r="A11" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="45" t="s">
+      <c r="D11" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="37" t="s">
-        <v>185</v>
+      <c r="E11" s="47" t="s">
+        <v>184</v>
       </c>
       <c r="F11" s="24" t="s">
         <v>40</v>
@@ -2124,11 +2119,11 @@
       <c r="J11" s="11"/>
     </row>
     <row r="12" spans="1:10" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="40"/>
-      <c r="B12" s="42"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="38"/>
+      <c r="A12" s="39"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="48"/>
       <c r="F12" s="24" t="s">
         <v>44</v>
       </c>
@@ -2169,12 +2164,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
@@ -2184,6 +2173,12 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:E7 E9:E11">
     <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
@@ -3376,7 +3371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0096DF0-D149-464A-950F-15761EF2F183}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -3439,7 +3434,9 @@
       <c r="D3" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>184</v>
+      </c>
       <c r="F3" s="4" t="s">
         <v>147</v>
       </c>
@@ -3644,6 +3641,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007916DAE6CBAB0E478E10A9FCA3CC0E19" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cc4eab9cdd79106b7ff0c84dd396c527">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="73b10483-4eab-47d9-97c6-997f49bd58aa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9c952eea70f5f85d64c583e57f778f77" ns2:_="">
     <xsd:import namespace="73b10483-4eab-47d9-97c6-997f49bd58aa"/>
@@ -3807,15 +3813,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -3823,6 +3820,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDA4E934-81D4-4CDA-A90D-B17985E7C5D3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF365504-DE0C-4D20-AADF-110855E1E7ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3840,14 +3845,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDA4E934-81D4-4CDA-A90D-B17985E7C5D3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D94FA3B0-7E84-4ED3-9FBD-9B6763F81478}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
page object model login, link
</commit_message>
<xml_diff>
--- a/DienmayXANH-TestData.xlsx
+++ b/DienmayXANH-TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phuong\eclipse-workspace\DienMayXanh\"/>
     </mc:Choice>
@@ -22,7 +22,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -544,16 +544,17 @@
     <t>Title</t>
   </si>
   <si>
+    <t>testLink</t>
+  </si>
+  <si>
     <t>PASSED</t>
-  </si>
-  <si>
-    <t>testLink</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1154,43 +1155,43 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1706,14 +1707,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="28.33203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="8" width="15.33203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="21.44140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="12.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="23.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="22.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="28.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="12.88671875" collapsed="true"/>
+    <col min="6" max="8" customWidth="true" style="1" width="15.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="21.44140625" collapsed="true"/>
+    <col min="10" max="16384" style="1" width="8.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1722,12 +1723,12 @@
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
       <c r="J1" s="11"/>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.35">
@@ -1879,13 +1880,13 @@
       <c r="J6" s="11"/>
     </row>
     <row r="7" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="39" t="s">
+      <c r="A7" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="45" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="42" t="s">
@@ -1909,9 +1910,9 @@
       <c r="J7" s="11"/>
     </row>
     <row r="8" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="38"/>
-      <c r="B8" s="39"/>
-      <c r="C8" s="41"/>
+      <c r="A8" s="37"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="48"/>
       <c r="D8" s="43"/>
       <c r="E8" s="4" t="s">
         <v>12</v>
@@ -1931,13 +1932,13 @@
       <c r="J8" s="11"/>
     </row>
     <row r="9" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="44" t="s">
+      <c r="A9" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="46" t="s">
+      <c r="C9" s="40" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="42" t="s">
@@ -1961,9 +1962,9 @@
       <c r="J9" s="11"/>
     </row>
     <row r="10" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="38"/>
-      <c r="B10" s="45"/>
-      <c r="C10" s="47"/>
+      <c r="A10" s="37"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="41"/>
       <c r="D10" s="43"/>
       <c r="E10" s="4" t="s">
         <v>12</v>
@@ -1983,13 +1984,13 @@
       <c r="J10" s="11"/>
     </row>
     <row r="11" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="48" t="s">
+      <c r="A11" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="45" t="s">
         <v>11</v>
       </c>
       <c r="D11" s="42" t="s">
@@ -2013,9 +2014,9 @@
       <c r="J11" s="11"/>
     </row>
     <row r="12" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="38"/>
-      <c r="B12" s="45"/>
-      <c r="C12" s="47"/>
+      <c r="A12" s="37"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="41"/>
       <c r="D12" s="43"/>
       <c r="E12" s="4" t="s">
         <v>12</v>
@@ -2060,6 +2061,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="C9:C10"/>
@@ -2068,11 +2074,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:E12">
     <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
@@ -2099,24 +2100,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="E4" sqref="E4:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.44140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="50.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.33203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="8.88671875" style="1" collapsed="1"/>
-    <col min="9" max="9" width="8.88671875" style="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="12.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="33.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="22.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="50.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="12.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="15.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="15.0" collapsed="true"/>
+    <col min="8" max="16384" style="1" width="8.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -2177,7 +2176,7 @@
         <v>52</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>51</v>
@@ -2198,7 +2197,7 @@
         <v>52</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>53</v>
@@ -2219,7 +2218,7 @@
         <v>52</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F6" s="33" t="s">
         <v>54</v>
@@ -2240,7 +2239,7 @@
         <v>52</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F7" s="33"/>
       <c r="G7" s="4"/>
@@ -2259,7 +2258,7 @@
         <v>52</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>55</v>
@@ -2280,7 +2279,7 @@
         <v>58</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F9" s="33" t="s">
         <v>56</v>
@@ -2303,7 +2302,7 @@
         <v>61</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F10" s="33" t="s">
         <v>59</v>
@@ -2326,7 +2325,7 @@
         <v>58</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F11" s="33" t="s">
         <v>62</v>
@@ -2349,7 +2348,7 @@
         <v>58</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F12" s="33" t="s">
         <v>64</v>
@@ -2372,7 +2371,7 @@
         <v>58</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F13" s="33" t="s">
         <v>66</v>
@@ -2395,7 +2394,7 @@
         <v>61</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F14" s="33" t="s">
         <v>68</v>
@@ -2416,7 +2415,7 @@
         <v>70</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F15" s="33" t="s">
         <v>69</v>
@@ -2452,7 +2451,7 @@
         <v>71</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
@@ -2516,14 +2515,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="44.44140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="28.33203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="9" width="15.33203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="21.44140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="16384" width="8.88671875" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="12.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="44.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="22.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="28.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="12.88671875" collapsed="true"/>
+    <col min="6" max="9" customWidth="true" style="1" width="15.33203125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="21.44140625" collapsed="true"/>
+    <col min="11" max="16384" style="1" width="8.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -2872,16 +2871,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.5546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.33203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="11.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="34.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="15.5546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="23.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="12.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="30.88671875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="17.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="9.88671875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="16.88671875" collapsed="true"/>
+    <col min="10" max="16384" style="1" width="8.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -3096,14 +3095,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="28.33203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.33203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="15" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="12.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="34.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="22.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="28.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="12.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="15.33203125" collapsed="true"/>
+    <col min="7" max="8" customWidth="true" style="1" width="15.0" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="8.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3295,15 +3294,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.5546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.44140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.33203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="30.109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="12.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="27.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="19.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="27.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="12.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="22.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="15.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="30.109375" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="8.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3393,23 +3392,21 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E3" sqref="E3:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.6640625" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="56" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="42.77734375" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="8.88671875" style="1" collapsed="1"/>
-    <col min="8" max="8" width="8.88671875" style="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="12.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="25.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="22.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="56.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="12.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="42.77734375" collapsed="true"/>
+    <col min="7" max="16384" style="1" width="8.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3442,7 +3439,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>11</v>
@@ -3451,7 +3448,7 @@
         <v>158</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F3" s="34" t="s">
         <v>153</v>
@@ -3462,7 +3459,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>11</v>
@@ -3471,7 +3468,7 @@
         <v>159</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F4" s="34" t="s">
         <v>154</v>
@@ -3482,7 +3479,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>11</v>
@@ -3491,7 +3488,7 @@
         <v>160</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F5" s="34" t="s">
         <v>155</v>
@@ -3502,7 +3499,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>11</v>
@@ -3511,7 +3508,7 @@
         <v>161</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F6" s="34" t="s">
         <v>156</v>
@@ -3522,7 +3519,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>11</v>
@@ -3531,7 +3528,7 @@
         <v>162</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F7" s="34" t="s">
         <v>157</v>
@@ -3733,18 +3730,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3766,18 +3763,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDA4E934-81D4-4CDA-A90D-B17985E7C5D3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D94FA3B0-7E84-4ED3-9FBD-9B6763F81478}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDA4E934-81D4-4CDA-A90D-B17985E7C5D3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
refactor all code for ChooseReceivedPlace and ViewProductThroughList
</commit_message>
<xml_diff>
--- a/DienmayXANH-TestData.xlsx
+++ b/DienmayXANH-TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3rdyears\autotestpractice\project\dienmayXANH\github\DienMayXanh\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3rdyears\autotest\project\dienmayXANH\github\DienMayXanh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADAC3FF1-A6B6-481D-9F61-1AA5C09EFE7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7741BCD-68B4-4425-A690-913D60DFF72E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ChooseReceivedPlace" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="186">
   <si>
     <t>Inputs</t>
   </si>
@@ -533,9 +533,6 @@
     <t>testSuccessViewProductByList</t>
   </si>
   <si>
-    <t>Máy lọc nước RO hydrogen ion kiềm Kangaroo 7 lõi KG100E0</t>
-  </si>
-  <si>
     <t>Hệ thống hiển thị đúng thông tin chi tiết sản phẩm đó</t>
   </si>
   <si>
@@ -594,6 +591,12 @@
   </si>
   <si>
     <t>PASSED</t>
+  </si>
+  <si>
+    <t>FAILED</t>
+  </si>
+  <si>
+    <t>Máy lọc nước RO hydrogen ion kiềm Kangaroo KG100E0</t>
   </si>
 </sst>
 </file>
@@ -1250,56 +1253,56 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1808,7 +1811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -1830,12 +1833,12 @@
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
       <c r="J1" s="11"/>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.35">
@@ -1882,7 +1885,7 @@
         <v>16</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F3" s="25" t="s">
         <v>12</v>
@@ -1903,7 +1906,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>11</v>
@@ -1912,7 +1915,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F4" s="24" t="s">
         <v>18</v>
@@ -1942,7 +1945,7 @@
         <v>23</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F5" s="24" t="s">
         <v>20</v>
@@ -1972,10 +1975,10 @@
         <v>27</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F6" s="31" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G6" s="24" t="s">
         <v>26</v>
@@ -1989,20 +1992,20 @@
       <c r="J6" s="11"/>
     </row>
     <row r="7" spans="1:10" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="40" t="s">
+      <c r="A7" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="43" t="s">
+      <c r="D7" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="45" t="s">
-        <v>184</v>
+      <c r="E7" s="52" t="s">
+        <v>183</v>
       </c>
       <c r="F7" s="28" t="s">
         <v>29</v>
@@ -2019,11 +2022,11 @@
       <c r="J7" s="11"/>
     </row>
     <row r="8" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="39"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="46"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="53"/>
       <c r="F8" s="26" t="s">
         <v>12</v>
       </c>
@@ -2039,20 +2042,20 @@
       <c r="J8" s="11"/>
     </row>
     <row r="9" spans="1:10" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="49" t="s">
+      <c r="A9" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="43" t="s">
+      <c r="D9" s="45" t="s">
         <v>38</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F9" s="29" t="s">
         <v>34</v>
@@ -2069,10 +2072,10 @@
       <c r="J9" s="11"/>
     </row>
     <row r="10" spans="1:10" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="39"/>
-      <c r="B10" s="50"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="44"/>
+      <c r="A10" s="40"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="46"/>
       <c r="E10" s="4"/>
       <c r="F10" s="32" t="s">
         <v>12</v>
@@ -2089,20 +2092,20 @@
       <c r="J10" s="11"/>
     </row>
     <row r="11" spans="1:10" ht="26" x14ac:dyDescent="0.35">
-      <c r="A11" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="53" t="s">
+      <c r="A11" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="41" t="s">
+      <c r="C11" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="43" t="s">
+      <c r="D11" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="47" t="s">
-        <v>184</v>
+      <c r="E11" s="37" t="s">
+        <v>183</v>
       </c>
       <c r="F11" s="24" t="s">
         <v>40</v>
@@ -2119,11 +2122,11 @@
       <c r="J11" s="11"/>
     </row>
     <row r="12" spans="1:10" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="39"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="48"/>
+      <c r="A12" s="40"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="38"/>
       <c r="F12" s="24" t="s">
         <v>44</v>
       </c>
@@ -2164,6 +2167,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
@@ -2173,12 +2182,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:E7 E9:E11">
     <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
@@ -3371,8 +3374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0096DF0-D149-464A-950F-15761EF2F183}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3432,10 +3435,10 @@
         <v>11</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>147</v>
@@ -3444,7 +3447,7 @@
         <v>148</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>164</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -3516,7 +3519,7 @@
         <v>47</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3524,17 +3527,17 @@
         <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="34" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3542,17 +3545,17 @@
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="34" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3560,17 +3563,17 @@
         <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="34" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3578,17 +3581,17 @@
         <v>9</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="34" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3596,17 +3599,17 @@
         <v>9</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="34" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -3641,15 +3644,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007916DAE6CBAB0E478E10A9FCA3CC0E19" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cc4eab9cdd79106b7ff0c84dd396c527">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="73b10483-4eab-47d9-97c6-997f49bd58aa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9c952eea70f5f85d64c583e57f778f77" ns2:_="">
     <xsd:import namespace="73b10483-4eab-47d9-97c6-997f49bd58aa"/>
@@ -3813,6 +3807,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -3820,14 +3823,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDA4E934-81D4-4CDA-A90D-B17985E7C5D3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF365504-DE0C-4D20-AADF-110855E1E7ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3845,6 +3840,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDA4E934-81D4-4CDA-A90D-B17985E7C5D3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D94FA3B0-7E84-4ED3-9FBD-9B6763F81478}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
complete view product through list
</commit_message>
<xml_diff>
--- a/DienmayXANH-TestData.xlsx
+++ b/DienmayXANH-TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\eclipse-workspace\DienmayXANH\DienMayXanh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84EACD59-5281-4D2E-86F4-6FE4C4B22175}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A601AD8A-7427-45CF-A241-6B0480B43511}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ChooseReceivedPlace" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="188">
   <si>
     <t>Inputs</t>
   </si>
@@ -536,12 +536,6 @@
     <t>testSuccessViewProductByList</t>
   </si>
   <si>
-    <t>Máy lọc nước RO hydrogen ion kiềm Kangaroo 7 lõi KG100E0</t>
-  </si>
-  <si>
-    <t>Hệ thống hiển thị đúng thông tin chi tiết sản phẩm đó</t>
-  </si>
-  <si>
     <t>Link_Facebook</t>
   </si>
   <si>
@@ -600,6 +594,12 @@
   </si>
   <si>
     <t>SORTING</t>
+  </si>
+  <si>
+    <t>Máy lọc nước RO hydrogen ion kiềm Kangaroo KG100E0</t>
+  </si>
+  <si>
+    <t>Máy lọc nước RO hydrogen ion kiềm Kangaroo KG100EO 7 lõi</t>
   </si>
   <si>
     <t>PASSED</t>
@@ -1113,7 +1113,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1223,49 +1223,58 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1776,7 +1785,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1797,12 +1806,12 @@
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
       <c r="J1" s="11"/>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.35">
@@ -1954,16 +1963,16 @@
       <c r="J6" s="11"/>
     </row>
     <row r="7" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="44" t="s">
+      <c r="A7" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="47" t="s">
+      <c r="D7" s="50" t="s">
         <v>31</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -1984,10 +1993,10 @@
       <c r="J7" s="11"/>
     </row>
     <row r="8" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="43"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="48"/>
+      <c r="A8" s="45"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="51"/>
       <c r="E8" s="4" t="s">
         <v>12</v>
       </c>
@@ -2006,16 +2015,16 @@
       <c r="J8" s="11"/>
     </row>
     <row r="9" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="49" t="s">
+      <c r="A9" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="47" t="s">
+      <c r="D9" s="50" t="s">
         <v>39</v>
       </c>
       <c r="E9" s="4" t="s">
@@ -2036,10 +2045,10 @@
       <c r="J9" s="11"/>
     </row>
     <row r="10" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="43"/>
-      <c r="B10" s="50"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="48"/>
+      <c r="A10" s="45"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="51"/>
       <c r="E10" s="4" t="s">
         <v>12</v>
       </c>
@@ -2058,16 +2067,16 @@
       <c r="J10" s="11"/>
     </row>
     <row r="11" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="53" t="s">
+      <c r="A11" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="47" t="s">
+      <c r="D11" s="50" t="s">
         <v>45</v>
       </c>
       <c r="E11" s="4" t="s">
@@ -2088,10 +2097,10 @@
       <c r="J11" s="11"/>
     </row>
     <row r="12" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="43"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="48"/>
+      <c r="A12" s="45"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="51"/>
       <c r="E12" s="4" t="s">
         <v>12</v>
       </c>
@@ -2135,6 +2144,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="C9:C10"/>
@@ -2143,11 +2157,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:E12">
     <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
@@ -2177,7 +2186,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2193,10 +2202,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="54" t="s">
+      <c r="F1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="54"/>
+      <c r="G1" s="57"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -2233,7 +2242,7 @@
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="42" t="s">
         <v>51</v>
       </c>
       <c r="G3" s="4"/>
@@ -2252,7 +2261,7 @@
         <v>54</v>
       </c>
       <c r="E4" s="4"/>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="43" t="s">
         <v>53</v>
       </c>
       <c r="G4" s="4"/>
@@ -2271,7 +2280,7 @@
         <v>54</v>
       </c>
       <c r="E5" s="4"/>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="43" t="s">
         <v>56</v>
       </c>
       <c r="G5" s="4"/>
@@ -2290,7 +2299,7 @@
         <v>54</v>
       </c>
       <c r="E6" s="4"/>
-      <c r="F6" s="33" t="s">
+      <c r="F6" s="42" t="s">
         <v>58</v>
       </c>
       <c r="G6" s="4"/>
@@ -2309,7 +2318,7 @@
         <v>54</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="F7" s="33"/>
+      <c r="F7" s="42"/>
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2326,7 +2335,7 @@
         <v>54</v>
       </c>
       <c r="E8" s="4"/>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="43" t="s">
         <v>61</v>
       </c>
       <c r="G8" s="4"/>
@@ -2345,7 +2354,7 @@
         <v>65</v>
       </c>
       <c r="E9" s="4"/>
-      <c r="F9" s="33" t="s">
+      <c r="F9" s="42" t="s">
         <v>63</v>
       </c>
       <c r="G9" s="33" t="s">
@@ -2366,7 +2375,7 @@
         <v>69</v>
       </c>
       <c r="E10" s="4"/>
-      <c r="F10" s="33" t="s">
+      <c r="F10" s="42" t="s">
         <v>67</v>
       </c>
       <c r="G10" s="33" t="s">
@@ -2387,7 +2396,7 @@
         <v>65</v>
       </c>
       <c r="E11" s="4"/>
-      <c r="F11" s="33" t="s">
+      <c r="F11" s="42" t="s">
         <v>71</v>
       </c>
       <c r="G11" s="33" t="s">
@@ -2408,7 +2417,7 @@
         <v>65</v>
       </c>
       <c r="E12" s="4"/>
-      <c r="F12" s="33" t="s">
+      <c r="F12" s="42" t="s">
         <v>74</v>
       </c>
       <c r="G12" s="33" t="s">
@@ -2429,7 +2438,7 @@
         <v>65</v>
       </c>
       <c r="E13" s="4"/>
-      <c r="F13" s="33" t="s">
+      <c r="F13" s="42" t="s">
         <v>77</v>
       </c>
       <c r="G13" s="4" t="s">
@@ -2450,7 +2459,7 @@
         <v>69</v>
       </c>
       <c r="E14" s="4"/>
-      <c r="F14" s="33" t="s">
+      <c r="F14" s="42" t="s">
         <v>80</v>
       </c>
       <c r="G14" s="4"/>
@@ -2469,7 +2478,7 @@
         <v>83</v>
       </c>
       <c r="E15" s="4"/>
-      <c r="F15" s="33" t="s">
+      <c r="F15" s="42" t="s">
         <v>82</v>
       </c>
       <c r="G15" s="4"/>
@@ -2486,7 +2495,7 @@
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
-      <c r="F16" s="33" t="s">
+      <c r="F16" s="42" t="s">
         <v>51</v>
       </c>
       <c r="G16" s="4"/>
@@ -2505,7 +2514,7 @@
         <v>86</v>
       </c>
       <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
+      <c r="F17" s="43"/>
       <c r="G17" s="4"/>
     </row>
   </sheetData>
@@ -2554,6 +2563,9 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="F3 F9 F6 F10:F16 G9:G11" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -2562,7 +2574,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H3" sqref="H3:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2578,13 +2590,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="55" t="s">
+      <c r="F1" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -2910,6 +2922,9 @@
     <hyperlink ref="J9" r:id="rId4" xr:uid="{BC5BFCF5-49B3-4927-9671-BE9437F7DF1A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="H3:H8" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -2918,7 +2933,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E3:E9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2936,12 +2951,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="57" t="s">
+      <c r="F1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
       <c r="J1" s="38"/>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2973,7 +2988,7 @@
         <v>92</v>
       </c>
       <c r="J2" s="37" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2989,9 +3004,7 @@
       <c r="D3" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>187</v>
-      </c>
+      <c r="E3" s="4"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5" t="s">
         <v>130</v>
@@ -3003,7 +3016,7 @@
         <v>132</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3019,9 +3032,7 @@
       <c r="D4" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>187</v>
-      </c>
+      <c r="E4" s="4"/>
       <c r="F4" s="5" t="s">
         <v>135</v>
       </c>
@@ -3035,7 +3046,7 @@
         <v>132</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.3">
@@ -3051,9 +3062,7 @@
       <c r="D5" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>187</v>
-      </c>
+      <c r="E5" s="4"/>
       <c r="F5" s="5" t="s">
         <v>137</v>
       </c>
@@ -3065,7 +3074,7 @@
         <v>132</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
@@ -3081,9 +3090,7 @@
       <c r="D6" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>187</v>
-      </c>
+      <c r="E6" s="4"/>
       <c r="F6" s="5" t="s">
         <v>137</v>
       </c>
@@ -3097,7 +3104,7 @@
         <v>132</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -3113,9 +3120,7 @@
       <c r="D7" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>187</v>
-      </c>
+      <c r="E7" s="4"/>
       <c r="F7" s="5" t="s">
         <v>142</v>
       </c>
@@ -3129,7 +3134,7 @@
         <v>132</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3173,8 +3178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86148902-2347-4FB2-AC60-64E22A6D30AB}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E5:E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3185,17 +3190,17 @@
     <col min="4" max="4" customWidth="true" style="1" width="28.33203125" collapsed="true"/>
     <col min="5" max="5" customWidth="true" style="1" width="12.88671875" collapsed="true"/>
     <col min="6" max="6" customWidth="true" style="1" width="15.33203125" collapsed="true"/>
-    <col min="7" max="9" customWidth="true" style="1" width="15.0" collapsed="true"/>
-    <col min="10" max="16384" style="1" width="8.88671875" collapsed="true"/>
+    <col min="7" max="8" customWidth="true" style="1" width="15.0" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="8.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="59" t="s">
+      <c r="F1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="40"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="39"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -3222,8 +3227,8 @@
       <c r="H2" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="I2" s="37" t="s">
-        <v>183</v>
+      <c r="I2" s="40" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3243,11 +3248,9 @@
       <c r="F3" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>149</v>
-      </c>
+      <c r="G3" s="4"/>
       <c r="H3" s="4"/>
-      <c r="I3" s="39"/>
+      <c r="I3" s="41"/>
     </row>
     <row r="4" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -3270,7 +3273,7 @@
         <v>149</v>
       </c>
       <c r="H4" s="4"/>
-      <c r="I4" s="39"/>
+      <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
@@ -3285,20 +3288,16 @@
       <c r="D5" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>187</v>
-      </c>
+      <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>149</v>
-      </c>
+      <c r="G5" s="4"/>
       <c r="H5" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="I5" s="39" t="s">
-        <v>186</v>
+      <c r="I5" s="41" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3314,20 +3313,16 @@
       <c r="D6" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>187</v>
-      </c>
+      <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>149</v>
-      </c>
+      <c r="G6" s="4"/>
       <c r="H6" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="I6" s="39" t="s">
-        <v>186</v>
+      <c r="I6" s="4" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3343,15 +3338,13 @@
       <c r="D7" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>187</v>
-      </c>
+      <c r="E7" s="4"/>
       <c r="F7" s="4" t="s">
         <v>148</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="39"/>
+      <c r="I7" s="41"/>
     </row>
     <row r="8" spans="1:9" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
@@ -3373,11 +3366,11 @@
       <formula>"PASSED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C7" xr:uid="{9762B304-547B-4610-970A-60696BA086F7}">
+  <dataValidations disablePrompts="1" count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C7" xr:uid="{9169F4EA-06C1-48AC-894C-C7BB8DC03F7F}">
       <formula1>"SUCCESSFULLY, UNSUCCESSFULLY"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E7" xr:uid="{7E6AC655-F6A0-4125-AE20-8D2983C308AE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E7" xr:uid="{A0357C4D-DA73-414B-9C4C-22193D19A787}">
       <formula1>"PASSED, FAILED, SKIPPED"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3389,8 +3382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0096DF0-D149-464A-950F-15761EF2F183}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3407,11 +3400,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="60" t="s">
+      <c r="F1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -3450,9 +3443,11 @@
         <v>11</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="E3" s="4"/>
+        <v>186</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>187</v>
+      </c>
       <c r="F3" s="4" t="s">
         <v>148</v>
       </c>
@@ -3460,7 +3455,7 @@
         <v>149</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>165</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -3532,7 +3527,7 @@
         <v>48</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3540,17 +3535,17 @@
         <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="34" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3558,17 +3553,17 @@
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="34" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3576,17 +3571,17 @@
         <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="34" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3594,17 +3589,17 @@
         <v>9</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="34" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3612,17 +3607,17 @@
         <v>9</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="34" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -3657,15 +3652,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007916DAE6CBAB0E478E10A9FCA3CC0E19" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cc4eab9cdd79106b7ff0c84dd396c527">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="73b10483-4eab-47d9-97c6-997f49bd58aa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9c952eea70f5f85d64c583e57f778f77" ns2:_="">
     <xsd:import namespace="73b10483-4eab-47d9-97c6-997f49bd58aa"/>
@@ -3829,6 +3815,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -3836,14 +3831,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDA4E934-81D4-4CDA-A90D-B17985E7C5D3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF365504-DE0C-4D20-AADF-110855E1E7ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3861,6 +3848,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDA4E934-81D4-4CDA-A90D-B17985E7C5D3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D94FA3B0-7E84-4ED3-9FBD-9B6763F81478}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
merge choose received place
</commit_message>
<xml_diff>
--- a/DienmayXANH-TestData.xlsx
+++ b/DienmayXANH-TestData.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\eclipse-workspace\DienmayXANH\DienMayXanh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D08B492-AAA1-49CC-BC6D-7D513195E8D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC00EEE1-9B8D-4D0C-8460-7D3B4C07A612}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ChooseReceivedPlace" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="199">
   <si>
     <t>Inputs</t>
   </si>
@@ -119,9 +119,6 @@
     <t>UNSUCCESSFULLY</t>
   </si>
   <si>
-    <t xml:space="preserve">Bình Định </t>
-  </si>
-  <si>
     <t>Huyện Vân Canh</t>
   </si>
   <si>
@@ -612,13 +609,39 @@
   </si>
   <si>
     <t>PASSED</t>
+  </si>
+  <si>
+    <t>testSuccessWithOnlyProvince</t>
+  </si>
+  <si>
+    <t>Bình Định</t>
+  </si>
+  <si>
+    <t>FULL_INFORMATION</t>
+  </si>
+  <si>
+    <t>ONLY_PROVINCE</t>
+  </si>
+  <si>
+    <t>NOT_FILL_ADDRESS</t>
+  </si>
+  <si>
+    <t>NOT_CHOOSE_WARD</t>
+  </si>
+  <si>
+    <t>UPDATE_ONLY_PROVINCE_SUBMIT_BEFORE</t>
+  </si>
+  <si>
+    <t>UPDATE_BY_CLICK_ON_BUTTON_CHANGE</t>
+  </si>
+  <si>
+    <t>UPDATE_BY_CLICK_ON_DROP_BOX_PROVINCE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -766,7 +789,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -1117,12 +1140,88 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1165,56 +1264,8 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1247,6 +1298,87 @@
     <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1270,6 +1402,12 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1812,39 +1950,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="12.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="23.88671875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="22.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="28.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="12.88671875" collapsed="true"/>
-    <col min="6" max="8" customWidth="true" style="1" width="15.33203125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="21.44140625" collapsed="true"/>
-    <col min="10" max="16384" style="1" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="12.109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.88671875" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="28.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.88671875" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="8" width="15.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="21.44140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="37.21875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11"/>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
-      <c r="F1" s="44" t="s">
+      <c r="F1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="11"/>
-    </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="11"/>
+    </row>
+    <row r="2" spans="1:11" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
@@ -1858,7 +1998,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F2" s="14" t="s">
         <v>4</v>
@@ -1872,283 +2012,292 @@
       <c r="I2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="15"/>
-    </row>
-    <row r="3" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="22" t="s">
+      <c r="J2" s="29" t="s">
+        <v>180</v>
+      </c>
+      <c r="K2" s="15"/>
+    </row>
+    <row r="3" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="32"/>
+      <c r="F3" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="G3" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="K3" s="11"/>
+    </row>
+    <row r="4" spans="1:11" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="C4" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="32"/>
+      <c r="F4" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="11"/>
-    </row>
-    <row r="4" spans="1:10" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="23" t="s">
+      <c r="H4" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="31" t="s">
+        <v>193</v>
+      </c>
+      <c r="K4" s="11"/>
+    </row>
+    <row r="5" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="32"/>
+      <c r="F5" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="31" t="s">
+        <v>194</v>
+      </c>
+      <c r="K5" s="11"/>
+    </row>
+    <row r="6" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="32"/>
+      <c r="F6" s="47" t="s">
+        <v>191</v>
+      </c>
+      <c r="G6" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="31" t="s">
+        <v>195</v>
+      </c>
+      <c r="K6" s="11"/>
+    </row>
+    <row r="7" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="59" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="63"/>
+      <c r="F7" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="50" t="s">
+        <v>196</v>
+      </c>
+      <c r="K7" s="11"/>
+    </row>
+    <row r="8" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="57"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" s="51"/>
+      <c r="K8" s="11"/>
+    </row>
+    <row r="9" spans="1:11" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="65" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="32"/>
+      <c r="F9" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" s="50" t="s">
+        <v>197</v>
+      </c>
+      <c r="K9" s="11"/>
+    </row>
+    <row r="10" spans="1:11" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="57"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" s="51"/>
+      <c r="K10" s="11"/>
+    </row>
+    <row r="11" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C11" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="24" t="s">
+      <c r="D11" s="61" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="53"/>
+      <c r="F11" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="J11" s="50" t="s">
+        <v>198</v>
+      </c>
+      <c r="K11" s="11"/>
+    </row>
+    <row r="12" spans="1:11" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="57"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H12" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I12" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="11"/>
-    </row>
-    <row r="5" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" s="11"/>
-    </row>
-    <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" s="11"/>
-    </row>
-    <row r="7" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="45" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="48" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="50" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" s="11"/>
-    </row>
-    <row r="8" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="46"/>
-      <c r="B8" s="47"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="I8" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" s="11"/>
-    </row>
-    <row r="9" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="45" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="52" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="54" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="50" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="H9" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="I9" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="J9" s="11"/>
-    </row>
-    <row r="10" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="46"/>
-      <c r="B10" s="53"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="I10" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="J10" s="11"/>
-    </row>
-    <row r="11" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="45" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="56" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="48" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="G11" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="H11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="I11" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="J11" s="11"/>
-    </row>
-    <row r="12" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="46"/>
-      <c r="B12" s="53"/>
-      <c r="C12" s="55"/>
-      <c r="D12" s="51"/>
-      <c r="E12" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="G12" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="I12" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="J12" s="11"/>
-    </row>
-    <row r="13" spans="1:10" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J12" s="52"/>
+      <c r="K12" s="11"/>
+    </row>
+    <row r="13" spans="1:11" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -2159,8 +2308,9 @@
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
-    </row>
-    <row r="14" spans="1:10" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K13" s="11"/>
+    </row>
+    <row r="14" spans="1:11" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
@@ -2171,9 +2321,10 @@
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="18">
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="C9:C10"/>
@@ -2182,20 +2333,25 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F1:I1"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:E12">
-    <cfRule type="cellIs" dxfId="29" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="4" operator="equal">
       <formula>"SKIPPED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="5" operator="equal">
       <formula>"FAILED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="6" operator="equal">
       <formula>"PASSED"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2208,6 +2364,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2221,21 +2378,21 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="12.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="35.44140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="22.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="50.88671875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="12.88671875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="15.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="15.0" collapsed="true"/>
-    <col min="8" max="16384" style="1" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="12.109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.44140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="50.88671875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.88671875" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="8.88671875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="57" t="s">
+      <c r="F1" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="57"/>
+      <c r="G1" s="70"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -2251,29 +2408,29 @@
         <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>49</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>50</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="42" t="s">
-        <v>51</v>
+      <c r="F3" s="26" t="s">
+        <v>50</v>
       </c>
       <c r="G3" s="4"/>
     </row>
@@ -2281,18 +2438,18 @@
       <c r="A4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="35" t="s">
-        <v>52</v>
+      <c r="B4" s="19" t="s">
+        <v>51</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E4" s="4"/>
-      <c r="F4" s="43" t="s">
-        <v>53</v>
+      <c r="F4" s="27" t="s">
+        <v>52</v>
       </c>
       <c r="G4" s="4"/>
     </row>
@@ -2301,17 +2458,17 @@
         <v>9</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E5" s="4"/>
-      <c r="F5" s="43" t="s">
-        <v>56</v>
+      <c r="F5" s="27" t="s">
+        <v>55</v>
       </c>
       <c r="G5" s="4"/>
     </row>
@@ -2320,17 +2477,17 @@
         <v>9</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E6" s="4"/>
-      <c r="F6" s="42" t="s">
-        <v>58</v>
+      <c r="F6" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="G6" s="4"/>
     </row>
@@ -2339,16 +2496,16 @@
         <v>9</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="F7" s="42"/>
+      <c r="F7" s="26"/>
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2356,17 +2513,17 @@
         <v>9</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E8" s="4"/>
-      <c r="F8" s="43" t="s">
-        <v>61</v>
+      <c r="F8" s="27" t="s">
+        <v>60</v>
       </c>
       <c r="G8" s="4"/>
     </row>
@@ -2375,20 +2532,20 @@
         <v>9</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E9" s="4"/>
-      <c r="F9" s="42" t="s">
+      <c r="F9" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="17" t="s">
         <v>63</v>
-      </c>
-      <c r="G9" s="33" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2396,20 +2553,20 @@
         <v>9</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E10" s="4"/>
-      <c r="F10" s="42" t="s">
+      <c r="F10" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" s="17" t="s">
         <v>67</v>
-      </c>
-      <c r="G10" s="33" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2417,20 +2574,20 @@
         <v>9</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E11" s="4"/>
-      <c r="F11" s="42" t="s">
+      <c r="F11" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="17" t="s">
         <v>71</v>
-      </c>
-      <c r="G11" s="33" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2438,20 +2595,20 @@
         <v>9</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E12" s="4"/>
-      <c r="F12" s="42" t="s">
+      <c r="F12" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G12" s="17" t="s">
         <v>74</v>
-      </c>
-      <c r="G12" s="33" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2459,20 +2616,20 @@
         <v>9</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E13" s="4"/>
-      <c r="F13" s="42" t="s">
+      <c r="F13" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2480,17 +2637,17 @@
         <v>9</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E14" s="4"/>
-      <c r="F14" s="42" t="s">
-        <v>80</v>
+      <c r="F14" s="26" t="s">
+        <v>79</v>
       </c>
       <c r="G14" s="4"/>
     </row>
@@ -2499,34 +2656,34 @@
         <v>9</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E15" s="4"/>
-      <c r="F15" s="42" t="s">
-        <v>82</v>
+      <c r="F15" s="26" t="s">
+        <v>81</v>
       </c>
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:7" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
-      <c r="F16" s="42" t="s">
-        <v>51</v>
+      <c r="F16" s="26" t="s">
+        <v>50</v>
       </c>
       <c r="G16" s="4"/>
     </row>
@@ -2535,16 +2692,16 @@
         <v>9</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E17" s="4"/>
-      <c r="F17" s="43"/>
+      <c r="F17" s="27"/>
       <c r="G17" s="4"/>
     </row>
   </sheetData>
@@ -2609,24 +2766,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="12.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="44.44140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="22.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="28.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="12.88671875" collapsed="true"/>
-    <col min="6" max="9" customWidth="true" style="1" width="15.33203125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="21.44140625" collapsed="true"/>
-    <col min="11" max="16384" style="1" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="12.109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="44.44140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="28.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.88671875" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="9" width="15.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="21.44140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="16384" width="8.88671875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="58" t="s">
-        <v>87</v>
-      </c>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
+      <c r="F1" s="71" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -2642,22 +2799,22 @@
         <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2665,29 +2822,29 @@
         <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="H3" s="33" t="s">
+      <c r="I3" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="I3" s="33" t="s">
+      <c r="J3" s="18" t="s">
         <v>97</v>
-      </c>
-      <c r="J3" s="34" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2695,111 +2852,111 @@
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="33" t="s">
-        <v>103</v>
+      <c r="D4" s="17" t="s">
+        <v>102</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G4" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="H4" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="H4" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="I4" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="J4" s="34"/>
+      <c r="I4" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="J4" s="18"/>
     </row>
     <row r="5" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G5" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H5" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="H5" s="33" t="s">
-        <v>106</v>
-      </c>
-      <c r="I5" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="J5" s="34"/>
+      <c r="I5" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="J5" s="18"/>
     </row>
     <row r="6" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G6" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H6" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="H6" s="33" t="s">
-        <v>109</v>
-      </c>
-      <c r="I6" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="J6" s="34"/>
+      <c r="I6" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="J6" s="18"/>
     </row>
     <row r="7" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="33" t="s">
-        <v>112</v>
+      <c r="D7" s="17" t="s">
+        <v>111</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="H7" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="I7" s="33"/>
-      <c r="J7" s="34" t="s">
-        <v>98</v>
+        <v>110</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="I7" s="17"/>
+      <c r="J7" s="18" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2807,27 +2964,27 @@
         <v>9</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="33" t="s">
-        <v>115</v>
+      <c r="D8" s="17" t="s">
+        <v>114</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G8" s="4"/>
-      <c r="H8" s="33" t="s">
-        <v>114</v>
-      </c>
-      <c r="I8" s="33" t="s">
+      <c r="H8" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="J8" s="18" t="s">
         <v>97</v>
-      </c>
-      <c r="J8" s="34" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2835,27 +2992,27 @@
         <v>9</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G9" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="H9" s="4"/>
+      <c r="I9" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="J9" s="18" t="s">
         <v>117</v>
-      </c>
-      <c r="H9" s="4"/>
-      <c r="I9" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="J9" s="34" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2863,27 +3020,27 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G10" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="J10" s="18" t="s">
         <v>121</v>
-      </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="J10" s="34" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2891,27 +3048,27 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="33" t="s">
-        <v>126</v>
+      <c r="D11" s="17" t="s">
+        <v>125</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G11" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="H11" s="4"/>
+      <c r="I11" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="J11" s="18" t="s">
         <v>124</v>
-      </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="J11" s="34" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -2963,31 +3120,31 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="11.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="34.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="15.5546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="23.88671875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="12.88671875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="30.88671875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="17.33203125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="9.88671875" collapsed="true"/>
-    <col min="9" max="10" customWidth="true" style="1" width="16.88671875" collapsed="true"/>
-    <col min="11" max="16384" style="1" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="11.109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.5546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.88671875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.88671875" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30.88671875" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.88671875" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="16.88671875" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="16384" width="8.88671875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="60" t="s">
+      <c r="F1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="38"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -3003,22 +3160,22 @@
         <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>128</v>
-      </c>
       <c r="I2" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="J2" s="37" t="s">
-        <v>181</v>
+        <v>91</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -3026,27 +3183,27 @@
         <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="I3" s="6" t="s">
-        <v>132</v>
-      </c>
       <c r="J3" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3054,29 +3211,29 @@
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G4" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="I4" s="6" t="s">
-        <v>132</v>
-      </c>
       <c r="J4" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.3">
@@ -3084,27 +3241,27 @@
         <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="I5" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="I5" s="6" t="s">
-        <v>132</v>
-      </c>
       <c r="J5" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
@@ -3112,29 +3269,29 @@
         <v>9</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H6" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="I6" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="I6" s="6" t="s">
-        <v>132</v>
-      </c>
       <c r="J6" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -3142,29 +3299,29 @@
         <v>9</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G7" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="I7" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="I7" s="6" t="s">
-        <v>132</v>
-      </c>
       <c r="J7" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3214,23 +3371,23 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="12.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="34.109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="22.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="28.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="12.88671875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="15.33203125" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" style="1" width="15.0" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="12.109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="28.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.88671875" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="15" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="62" t="s">
+      <c r="F1" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="39"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="23"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -3246,19 +3403,19 @@
         <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="I2" s="40" t="s">
-        <v>181</v>
+      <c r="I2" s="24" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3266,41 +3423,41 @@
         <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
-      <c r="I3" s="41"/>
+      <c r="I3" s="25"/>
     </row>
     <row r="4" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>148</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>149</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -3310,24 +3467,24 @@
         <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="I5" s="41" t="s">
-        <v>184</v>
+        <v>153</v>
+      </c>
+      <c r="I5" s="25" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3335,24 +3492,24 @@
         <v>9</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3360,25 +3517,25 @@
         <v>9</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="41"/>
+      <c r="I7" s="25"/>
     </row>
     <row r="8" spans="1:9" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -3412,29 +3569,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0096DF0-D149-464A-950F-15761EF2F183}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="12.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="27.5546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="19.44140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="27.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="12.88671875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="22.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="15.33203125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="30.109375" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="12.109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.5546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.44140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="27.109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.88671875" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="30.109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="63" t="s">
+      <c r="F1" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -3450,68 +3607,68 @@
         <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="H2" s="3" t="s">
+    </row>
+    <row r="3" spans="1:8" s="16" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>163</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="27" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>164</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>149</v>
-      </c>
       <c r="H3" s="5" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="27" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="16" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>190</v>
-      </c>
       <c r="F4" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>187</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -3563,17 +3720,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="12.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="25.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="22.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="35.88671875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="12.88671875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="42.77734375" collapsed="true"/>
-    <col min="7" max="16384" style="1" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="12.109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.6640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="35.88671875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.88671875" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="42.77734375" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="20" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3591,10 +3748,10 @@
         <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3602,17 +3759,17 @@
         <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E3" s="4"/>
-      <c r="F3" s="34" t="s">
-        <v>176</v>
+      <c r="F3" s="18" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3620,17 +3777,17 @@
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E4" s="4"/>
-      <c r="F4" s="34" t="s">
-        <v>177</v>
+      <c r="F4" s="18" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3638,17 +3795,17 @@
         <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E5" s="4"/>
-      <c r="F5" s="34" t="s">
-        <v>178</v>
+      <c r="F5" s="18" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3656,17 +3813,17 @@
         <v>9</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E6" s="4"/>
-      <c r="F6" s="34" t="s">
-        <v>179</v>
+      <c r="F6" s="18" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3674,17 +3831,17 @@
         <v>9</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="F7" s="34" t="s">
-        <v>180</v>
+      <c r="F7" s="18" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -3719,15 +3876,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007916DAE6CBAB0E478E10A9FCA3CC0E19" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cc4eab9cdd79106b7ff0c84dd396c527">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="73b10483-4eab-47d9-97c6-997f49bd58aa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9c952eea70f5f85d64c583e57f778f77" ns2:_="">
     <xsd:import namespace="73b10483-4eab-47d9-97c6-997f49bd58aa"/>
@@ -3891,6 +4039,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -3898,14 +4055,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDA4E934-81D4-4CDA-A90D-B17985E7C5D3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF365504-DE0C-4D20-AADF-110855E1E7ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3923,6 +4072,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDA4E934-81D4-4CDA-A90D-B17985E7C5D3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D94FA3B0-7E84-4ED3-9FBD-9B6763F81478}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
complete choose received place
</commit_message>
<xml_diff>
--- a/DienmayXANH-TestData.xlsx
+++ b/DienmayXANH-TestData.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\eclipse-workspace\DienmayXANH\DienMayXanh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC00EEE1-9B8D-4D0C-8460-7D3B4C07A612}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F92627E-2FAB-48F6-813E-945B5DA295F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="221">
   <si>
     <t>Inputs</t>
   </si>
@@ -636,12 +636,79 @@
   </si>
   <si>
     <t>UPDATE_BY_CLICK_ON_DROP_BOX_PROVINCE</t>
+  </si>
+  <si>
+    <t>Quận 10</t>
+  </si>
+  <si>
+    <t>Phường 01</t>
+  </si>
+  <si>
+    <t>418 Lê Hồng Phong</t>
+  </si>
+  <si>
+    <t>418 Lê Hồng Phong, Phường 01, Quận 10, Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>Bến Tre</t>
+  </si>
+  <si>
+    <t>Phường 01, Quận 10, Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>Quận Cẩm Lệ</t>
+  </si>
+  <si>
+    <t>Quảng Ninh</t>
+  </si>
+  <si>
+    <t>TP. Móng Cái</t>
+  </si>
+  <si>
+    <t>Phường Hải Yên</t>
+  </si>
+  <si>
+    <t>Phường Hải Yên, TP. Móng Cái, Quảng Ninh</t>
+  </si>
+  <si>
+    <t>Quảng Ngãi</t>
+  </si>
+  <si>
+    <t>Huyện Ba Tơ</t>
+  </si>
+  <si>
+    <t>Thị trấn Ba Tơ</t>
+  </si>
+  <si>
+    <t>123 Ba Tơ</t>
+  </si>
+  <si>
+    <t>321 Ba Tơ</t>
+  </si>
+  <si>
+    <t>321 Ba Tơ, Thị trấn Ba Tơ, Huyện Ba Tơ, Quảng Ngãi</t>
+  </si>
+  <si>
+    <t>Bình Dương</t>
+  </si>
+  <si>
+    <t>Huyện Dầu Tiếng</t>
+  </si>
+  <si>
+    <t>Xã An Lập</t>
+  </si>
+  <si>
+    <t>123 An Lập</t>
+  </si>
+  <si>
+    <t>Cà Mau</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -909,19 +976,6 @@
       <right style="thin">
         <color rgb="FFFFFFFF"/>
       </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color rgb="FFFFFFFF"/>
@@ -998,30 +1052,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color theme="0"/>
       </left>
       <right/>
@@ -1216,12 +1246,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1264,7 +1331,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1304,125 +1371,140 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1453,7 +1535,49 @@
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="36">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF8064A2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF8064A2"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1950,23 +2074,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="28.33203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="8" width="15.33203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="21.44140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="37.21875" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="12.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="23.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="22.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="28.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="12.88671875" collapsed="true"/>
+    <col min="6" max="8" customWidth="true" style="1" width="15.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="21.44140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="37.21875" collapsed="false"/>
+    <col min="11" max="16384" style="1" width="8.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1975,12 +2099,12 @@
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
-      <c r="F1" s="55" t="s">
+      <c r="F1" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
       <c r="J1" s="28"/>
       <c r="K1" s="11"/>
     </row>
@@ -2018,32 +2142,34 @@
       <c r="K2" s="15"/>
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="39" t="s">
+      <c r="A3" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="46" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="32"/>
-      <c r="F3" s="42" t="s">
+      <c r="E3" s="51" t="s">
+        <v>189</v>
+      </c>
+      <c r="F3" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="42" t="s">
+      <c r="G3" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="42" t="s">
+      <c r="H3" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="42" t="s">
+      <c r="I3" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="30" t="s">
+      <c r="J3" s="52" t="s">
         <v>192</v>
       </c>
       <c r="K3" s="11"/>
@@ -2052,29 +2178,31 @@
       <c r="A4" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="37" t="s">
         <v>190</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="32"/>
-      <c r="F4" s="41" t="s">
+      <c r="E4" s="48" t="s">
+        <v>189</v>
+      </c>
+      <c r="F4" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="41" t="s">
+      <c r="G4" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="41" t="s">
+      <c r="H4" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="41" t="s">
+      <c r="I4" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="31" t="s">
+      <c r="J4" s="30" t="s">
         <v>193</v>
       </c>
       <c r="K4" s="11"/>
@@ -2083,26 +2211,28 @@
       <c r="A5" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="32"/>
-      <c r="F5" s="41" t="s">
+      <c r="E5" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="F5" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="41" t="s">
+      <c r="G5" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="41" t="s">
+      <c r="H5" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="41" t="s">
+      <c r="I5" s="38" t="s">
         <v>12</v>
       </c>
       <c r="J5" s="31" t="s">
@@ -2114,26 +2244,28 @@
       <c r="A6" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="47" t="s">
+      <c r="E6" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="F6" s="43" t="s">
         <v>191</v>
       </c>
-      <c r="G6" s="41" t="s">
+      <c r="G6" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="41" t="s">
+      <c r="H6" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="41" t="s">
+      <c r="I6" s="38" t="s">
         <v>12</v>
       </c>
       <c r="J6" s="31" t="s">
@@ -2142,189 +2274,482 @@
       <c r="K6" s="11"/>
     </row>
     <row r="7" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="56" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="58" t="s">
+      <c r="A7" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="64" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="63"/>
-      <c r="F7" s="44" t="s">
+      <c r="E7" s="67" t="s">
+        <v>189</v>
+      </c>
+      <c r="F7" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="41" t="s">
+      <c r="G7" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="41" t="s">
+      <c r="H7" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="41" t="s">
+      <c r="I7" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="50" t="s">
+      <c r="J7" s="69" t="s">
         <v>196</v>
       </c>
       <c r="K7" s="11"/>
     </row>
     <row r="8" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="57"/>
-      <c r="B8" s="58"/>
-      <c r="C8" s="60"/>
+      <c r="A8" s="56"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="66"/>
       <c r="D8" s="62"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="49" t="s">
+      <c r="E8" s="68"/>
+      <c r="F8" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="43" t="s">
+      <c r="G8" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="43" t="s">
+      <c r="H8" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="I8" s="41" t="s">
+      <c r="I8" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="51"/>
+      <c r="J8" s="70"/>
       <c r="K8" s="11"/>
     </row>
     <row r="9" spans="1:11" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="56" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="65" t="s">
+      <c r="A9" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="67" t="s">
+      <c r="C9" s="59" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="32"/>
-      <c r="F9" s="45" t="s">
+      <c r="E9" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="F9" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="46" t="s">
+      <c r="G9" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="H9" s="44" t="s">
+      <c r="H9" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="I9" s="41" t="s">
+      <c r="I9" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="J9" s="50" t="s">
+      <c r="J9" s="69" t="s">
         <v>197</v>
       </c>
       <c r="K9" s="11"/>
     </row>
     <row r="10" spans="1:11" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="57"/>
-      <c r="B10" s="66"/>
-      <c r="C10" s="68"/>
+      <c r="A10" s="56"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="60"/>
       <c r="D10" s="62"/>
       <c r="E10" s="32"/>
-      <c r="F10" s="48" t="s">
+      <c r="F10" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="41" t="s">
+      <c r="G10" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="41" t="s">
+      <c r="H10" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="41" t="s">
+      <c r="I10" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="J10" s="51"/>
+      <c r="J10" s="70"/>
       <c r="K10" s="11"/>
     </row>
     <row r="11" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="56" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="69" t="s">
+      <c r="A11" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="59" t="s">
+      <c r="C11" s="64" t="s">
         <v>11</v>
       </c>
       <c r="D11" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="53"/>
-      <c r="F11" s="41" t="s">
+      <c r="E11" s="72" t="s">
+        <v>189</v>
+      </c>
+      <c r="F11" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="G11" s="41" t="s">
+      <c r="G11" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="H11" s="41" t="s">
+      <c r="H11" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="I11" s="41" t="s">
+      <c r="I11" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="J11" s="50" t="s">
+      <c r="J11" s="69" t="s">
         <v>198</v>
       </c>
       <c r="K11" s="11"/>
     </row>
     <row r="12" spans="1:11" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="57"/>
-      <c r="B12" s="69"/>
-      <c r="C12" s="68"/>
+      <c r="A12" s="56"/>
+      <c r="B12" s="63"/>
+      <c r="C12" s="60"/>
       <c r="D12" s="62"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="41" t="s">
+      <c r="E12" s="73"/>
+      <c r="F12" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="G12" s="41" t="s">
+      <c r="G12" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="41" t="s">
+      <c r="H12" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="41" t="s">
+      <c r="I12" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="J12" s="52"/>
+      <c r="J12" s="71"/>
       <c r="K12" s="11"/>
     </row>
-    <row r="13" spans="1:11" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
+    <row r="13" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>202</v>
+      </c>
+      <c r="E13" s="51" t="s">
+        <v>189</v>
+      </c>
+      <c r="F13" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="38" t="s">
+        <v>199</v>
+      </c>
+      <c r="H13" s="38" t="s">
+        <v>200</v>
+      </c>
+      <c r="I13" s="38" t="s">
+        <v>201</v>
+      </c>
+      <c r="J13" s="52" t="s">
+        <v>192</v>
+      </c>
       <c r="K13" s="11"/>
     </row>
-    <row r="14" spans="1:11" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
+    <row r="14" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="C14" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>203</v>
+      </c>
+      <c r="E14" s="48" t="s">
+        <v>189</v>
+      </c>
+      <c r="F14" s="38" t="s">
+        <v>203</v>
+      </c>
+      <c r="G14" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="J14" s="30" t="s">
+        <v>193</v>
+      </c>
       <c r="K14" s="11"/>
     </row>
+    <row r="15" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>204</v>
+      </c>
+      <c r="E15" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="F15" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="38" t="s">
+        <v>199</v>
+      </c>
+      <c r="H15" s="38" t="s">
+        <v>200</v>
+      </c>
+      <c r="I15" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="J15" s="31" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="F16" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="38" t="s">
+        <v>205</v>
+      </c>
+      <c r="H16" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="J16" s="31" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="64" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="61" t="s">
+        <v>209</v>
+      </c>
+      <c r="E17" s="67" t="s">
+        <v>189</v>
+      </c>
+      <c r="F17" s="40" t="s">
+        <v>206</v>
+      </c>
+      <c r="G17" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="J17" s="69" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="56"/>
+      <c r="B18" s="65"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="62"/>
+      <c r="E18" s="68"/>
+      <c r="F18" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="39" t="s">
+        <v>207</v>
+      </c>
+      <c r="H18" s="39" t="s">
+        <v>208</v>
+      </c>
+      <c r="I18" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="J18" s="70"/>
+    </row>
+    <row r="19" spans="1:10" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="59" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="61" t="s">
+        <v>215</v>
+      </c>
+      <c r="E19" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="F19" s="41" t="s">
+        <v>210</v>
+      </c>
+      <c r="G19" s="42" t="s">
+        <v>211</v>
+      </c>
+      <c r="H19" s="40" t="s">
+        <v>212</v>
+      </c>
+      <c r="I19" s="38" t="s">
+        <v>213</v>
+      </c>
+      <c r="J19" s="69" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="56"/>
+      <c r="B20" s="58"/>
+      <c r="C20" s="60"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="I20" s="38" t="s">
+        <v>214</v>
+      </c>
+      <c r="J20" s="70"/>
+    </row>
+    <row r="21" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A21" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="64" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="61" t="s">
+        <v>220</v>
+      </c>
+      <c r="E21" s="72" t="s">
+        <v>189</v>
+      </c>
+      <c r="F21" s="38" t="s">
+        <v>216</v>
+      </c>
+      <c r="G21" s="38" t="s">
+        <v>217</v>
+      </c>
+      <c r="H21" s="38" t="s">
+        <v>218</v>
+      </c>
+      <c r="I21" s="38" t="s">
+        <v>219</v>
+      </c>
+      <c r="J21" s="69" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A22" s="56"/>
+      <c r="B22" s="63"/>
+      <c r="C22" s="60"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="38" t="s">
+        <v>220</v>
+      </c>
+      <c r="G22" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="I22" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="J22" s="71"/>
+    </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="35">
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="C9:C10"/>
@@ -2333,33 +2758,45 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:D12"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:E12">
-    <cfRule type="cellIs" dxfId="29" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="10" operator="equal">
       <formula>"SKIPPED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="11" operator="equal">
       <formula>"FAILED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="12" operator="equal">
+      <formula>"PASSED"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
+      <formula>"SKIPPED"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
+      <formula>"FAILED"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="6" operator="equal">
+      <formula>"PASSED"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14:E22">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"SKIPPED"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"FAILED"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"PASSED"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C12" xr:uid="{7CB3CA1F-9DC0-4F78-82D3-04616222504A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C22" xr:uid="{7CB3CA1F-9DC0-4F78-82D3-04616222504A}">
       <formula1>"SUCCESSFULLY, UNSUCCESSFULLY"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E12" xr:uid="{AF7DDB1A-CDEA-446A-A195-0F21E6E7FDE6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E22" xr:uid="{AF7DDB1A-CDEA-446A-A195-0F21E6E7FDE6}">
       <formula1>"PASSED, FAILED, SKIPPED"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2378,21 +2815,21 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.44140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="50.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.33203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="12.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="35.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="22.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="50.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="12.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="15.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="15.0" collapsed="true"/>
+    <col min="8" max="16384" style="1" width="8.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="70" t="s">
+      <c r="F1" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="70"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -2709,35 +3146,35 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:E15">
-    <cfRule type="cellIs" dxfId="26" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="7" operator="equal">
       <formula>"SKIPPED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="8" operator="equal">
       <formula>"FAILED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="9" operator="equal">
       <formula>"PASSED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="cellIs" dxfId="23" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="4" operator="equal">
       <formula>"SKIPPED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="5" operator="equal">
       <formula>"FAILED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="6" operator="equal">
       <formula>"PASSED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
       <formula>"SKIPPED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
       <formula>"FAILED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
       <formula>"PASSED"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2766,24 +3203,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="44.44140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="28.33203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="9" width="15.33203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="21.44140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="16384" width="8.88671875" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="12.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="44.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="22.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="28.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="12.88671875" collapsed="true"/>
+    <col min="6" max="9" customWidth="true" style="1" width="15.33203125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="21.44140625" collapsed="true"/>
+    <col min="11" max="16384" style="1" width="8.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="71" t="s">
+      <c r="F1" s="76" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -3084,13 +3521,13 @@
     <mergeCell ref="F1:J1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:E11">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
       <formula>"SKIPPED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
       <formula>"FAILED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
       <formula>"PASSED"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3125,25 +3562,25 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.5546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.33203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="10" width="16.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="16384" width="8.88671875" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="11.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="34.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="15.5546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="23.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="12.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="30.88671875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="17.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="9.88671875" collapsed="true"/>
+    <col min="9" max="10" customWidth="true" style="1" width="16.88671875" collapsed="true"/>
+    <col min="11" max="16384" style="1" width="8.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="73" t="s">
+      <c r="F1" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
       <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3332,13 +3769,13 @@
     <mergeCell ref="F1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:E7">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
       <formula>"SKIPPED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
       <formula>"FAILED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
       <formula>"PASSED"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3371,22 +3808,22 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="28.33203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.33203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="15" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="12.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="34.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="22.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="28.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="12.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="15.33203125" collapsed="true"/>
+    <col min="7" max="8" customWidth="true" style="1" width="15.0" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="8.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="75" t="s">
+      <c r="F1" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
       <c r="I1" s="23"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3543,13 +3980,13 @@
     <mergeCell ref="F1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:E7">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
       <formula>"SKIPPED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
       <formula>"FAILED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
       <formula>"PASSED"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3575,23 +4012,23 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.5546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.44140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.33203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="30.109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="12.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="27.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="19.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="27.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="12.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="22.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="15.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="30.109375" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="8.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="76" t="s">
+      <c r="F1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -3676,24 +4113,24 @@
     <mergeCell ref="F1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
       <formula>"SKIPPED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
       <formula>"FAILED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
       <formula>"PASSED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"SKIPPED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"FAILED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"PASSED"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3720,13 +4157,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.6640625" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="35.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="42.77734375" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="8.88671875" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="12.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="25.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="22.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="35.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="12.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="42.77734375" collapsed="true"/>
+    <col min="7" max="16384" style="1" width="8.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3846,13 +4283,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E3:E7">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"SKIPPED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"FAILED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"PASSED"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3876,6 +4313,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007916DAE6CBAB0E478E10A9FCA3CC0E19" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cc4eab9cdd79106b7ff0c84dd396c527">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="73b10483-4eab-47d9-97c6-997f49bd58aa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9c952eea70f5f85d64c583e57f778f77" ns2:_="">
     <xsd:import namespace="73b10483-4eab-47d9-97c6-997f49bd58aa"/>
@@ -4039,22 +4491,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D94FA3B0-7E84-4ED3-9FBD-9B6763F81478}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDA4E934-81D4-4CDA-A90D-B17985E7C5D3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF365504-DE0C-4D20-AADF-110855E1E7ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4070,21 +4524,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDA4E934-81D4-4CDA-A90D-B17985E7C5D3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D94FA3B0-7E84-4ED3-9FBD-9B6763F81478}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
completed refactor for login and link
</commit_message>
<xml_diff>
--- a/DienmayXANH-TestData.xlsx
+++ b/DienmayXANH-TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\eclipse-workspace\DienmayXANH\DienMayXanh\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3rdyears\autotest\project\dienmayXANH\github\DienMayXanh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D08B492-AAA1-49CC-BC6D-7D513195E8D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07CC532-067C-4CB8-BE5A-BA05685AF79B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ChooseReceivedPlace" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="177">
   <si>
     <t>Inputs</t>
   </si>
@@ -191,45 +191,24 @@
     <t>MANUAL</t>
   </si>
   <si>
-    <t>Login_Successfully</t>
-  </si>
-  <si>
     <t>0353266815</t>
   </si>
   <si>
-    <t>Login_PhoneNumbersWithLetters</t>
-  </si>
-  <si>
     <t>090dwwwr</t>
   </si>
   <si>
     <t>Số điện thoại trống/không đúng định dạng</t>
   </si>
   <si>
-    <t>Login_PhoneNumberWithSpecialCharacters</t>
-  </si>
-  <si>
     <t>575(){'.</t>
   </si>
   <si>
-    <t>Login_WrongPhoneNumber</t>
-  </si>
-  <si>
     <t>5412368521</t>
   </si>
   <si>
-    <t>Login_DoNotEnterPhoneNumber</t>
-  </si>
-  <si>
-    <t>Login_EnterSpace</t>
-  </si>
-  <si>
     <t xml:space="preserve">     </t>
   </si>
   <si>
-    <t>Login_WrongOTP</t>
-  </si>
-  <si>
     <t>0342256477</t>
   </si>
   <si>
@@ -239,9 +218,6 @@
     <t>* Mã xác nhận không đúng, vui lòng thử lại.</t>
   </si>
   <si>
-    <t>Login_DoNotEnterEnoughOTP</t>
-  </si>
-  <si>
     <t>0348775124</t>
   </si>
   <si>
@@ -251,54 +227,33 @@
     <t>* Vui lòng nhập mã OTP.</t>
   </si>
   <si>
-    <t>Login_OTPHasLetters</t>
-  </si>
-  <si>
     <t>0341235789</t>
   </si>
   <si>
     <t>45a2</t>
   </si>
   <si>
-    <t>Login_OTPHasSpecialCharacters</t>
-  </si>
-  <si>
     <t>0386586541</t>
   </si>
   <si>
     <t>4&gt;?2</t>
   </si>
   <si>
-    <t>Login_OTPEntersSpace</t>
-  </si>
-  <si>
     <t>0345154856</t>
   </si>
   <si>
     <t xml:space="preserve">    </t>
   </si>
   <si>
-    <t>Login_DoNotEnterOTP</t>
-  </si>
-  <si>
     <t>0389852132</t>
   </si>
   <si>
-    <t>Login_NoticeOfResendingOTP</t>
-  </si>
-  <si>
     <t>0345468365</t>
   </si>
   <si>
     <t>Tôi không nhận được mã, vui lòng gửi lại</t>
   </si>
   <si>
-    <t>Login_EnterKey</t>
-  </si>
-  <si>
-    <t>Login_Title</t>
-  </si>
-  <si>
     <t>Lịch sử mua hàng | Dienmayxanh.com | Dienmayxanh.com</t>
   </si>
   <si>
@@ -536,36 +491,6 @@
     <t>testSuccessViewProductByList</t>
   </si>
   <si>
-    <t>Link_Facebook</t>
-  </si>
-  <si>
-    <t>Hệ thống mở tab Facebook Điện máy xanh.</t>
-  </si>
-  <si>
-    <t>Link_Youtube</t>
-  </si>
-  <si>
-    <t>Hệ thống mở tab YouTube Điện máy xanh.</t>
-  </si>
-  <si>
-    <t>Link_MaiAm</t>
-  </si>
-  <si>
-    <t>Hệ thống mở tab MÁI ẤM Thế Giới Di Động.</t>
-  </si>
-  <si>
-    <t>Link_TGDD</t>
-  </si>
-  <si>
-    <t>Hệ thống mở tab thegioididong.com.</t>
-  </si>
-  <si>
-    <t>Link_BachHoaXanh</t>
-  </si>
-  <si>
-    <t>Hệ thống mở tab Bách hóa XANH.</t>
-  </si>
-  <si>
     <t>Link</t>
   </si>
   <si>
@@ -612,13 +537,45 @@
   </si>
   <si>
     <t>PASSED</t>
+  </si>
+  <si>
+    <t>TestName</t>
+  </si>
+  <si>
+    <t>LoginWithWrongFormatPhoneNumber</t>
+  </si>
+  <si>
+    <t>LoginWithWrongOTP</t>
+  </si>
+  <si>
+    <t>NoticeOfResendingOTP</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>testLink</t>
+  </si>
+  <si>
+    <t>Điện máy XANH (dienmayxanh.com) - Trang chủ | Facebook</t>
+  </si>
+  <si>
+    <t>Điện máy XANH - YouTube</t>
+  </si>
+  <si>
+    <t>Trang chủ - Mái Ấm TGDD</t>
+  </si>
+  <si>
+    <t>Thegioididong.com - Điện thoại, Laptop, Phụ kiện, Đồng hồ chính hãng</t>
+  </si>
+  <si>
+    <t>Siêu thị Bách hoá XANH - Mua bán thực phẩm, sản phẩm gia đình</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1122,7 +1079,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1148,142 +1105,155 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1818,362 +1788,367 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="12.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="23.88671875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="22.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="28.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="12.88671875" collapsed="true"/>
-    <col min="6" max="8" customWidth="true" style="1" width="15.33203125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="21.44140625" collapsed="true"/>
-    <col min="10" max="16384" style="1" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="12.08984375" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.90625" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="28.36328125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.90625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="8" width="15.36328125" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="21.453125" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="16384" width="8.90625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11"/>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="44" t="s">
+    <row r="1" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="11"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="15"/>
-    </row>
-    <row r="3" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="22" t="s">
+      <c r="J2" s="13"/>
+    </row>
+    <row r="3" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="15" t="s">
         <v>16</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="25" t="s">
+      <c r="I3" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="11"/>
-    </row>
-    <row r="4" spans="1:10" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="23" t="s">
+      <c r="J3" s="9"/>
+    </row>
+    <row r="4" spans="1:10" ht="27.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="16" t="s">
         <v>18</v>
       </c>
       <c r="E4" s="4"/>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="11"/>
-    </row>
-    <row r="5" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="23" t="s">
+      <c r="J4" s="9"/>
+    </row>
+    <row r="5" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="16" t="s">
         <v>23</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="24" t="s">
+      <c r="G5" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="24" t="s">
+      <c r="H5" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="24" t="s">
+      <c r="I5" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="11"/>
-    </row>
-    <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="23" t="s">
+      <c r="J5" s="9"/>
+    </row>
+    <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="16" t="s">
         <v>28</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="31" t="s">
+      <c r="F6" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="G6" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="H6" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="24" t="s">
+      <c r="I6" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="11"/>
-    </row>
-    <row r="7" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="45" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="47" t="s">
+      <c r="J6" s="9"/>
+    </row>
+    <row r="7" spans="1:10" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="50" t="s">
+      <c r="D7" s="55" t="s">
         <v>31</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="28" t="s">
+      <c r="F7" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="24" t="s">
+      <c r="G7" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="24" t="s">
+      <c r="H7" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="24" t="s">
+      <c r="I7" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="11"/>
-    </row>
-    <row r="8" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="46"/>
-      <c r="B8" s="47"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="51"/>
+      <c r="J7" s="9"/>
+    </row>
+    <row r="8" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="50"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="56"/>
       <c r="E8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="26" t="s">
+      <c r="G8" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="26" t="s">
+      <c r="H8" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="24" t="s">
+      <c r="I8" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="11"/>
-    </row>
-    <row r="9" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="45" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="52" t="s">
+      <c r="J8" s="9"/>
+    </row>
+    <row r="9" spans="1:10" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="54" t="s">
+      <c r="C9" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="50" t="s">
+      <c r="D9" s="55" t="s">
         <v>39</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="29" t="s">
+      <c r="F9" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="30" t="s">
+      <c r="G9" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="28" t="s">
+      <c r="H9" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="I9" s="24" t="s">
+      <c r="I9" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="J9" s="11"/>
-    </row>
-    <row r="10" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="46"/>
-      <c r="B10" s="53"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="51"/>
+      <c r="J9" s="9"/>
+    </row>
+    <row r="10" spans="1:10" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="50"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="56"/>
       <c r="E10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="32" t="s">
+      <c r="F10" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="24" t="s">
+      <c r="G10" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="24" t="s">
+      <c r="H10" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="24" t="s">
+      <c r="I10" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="J10" s="11"/>
-    </row>
-    <row r="11" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="45" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="56" t="s">
+      <c r="J10" s="9"/>
+    </row>
+    <row r="11" spans="1:10" ht="26" x14ac:dyDescent="0.35">
+      <c r="A11" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="50" t="s">
+      <c r="D11" s="55" t="s">
         <v>45</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="24" t="s">
+      <c r="F11" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="24" t="s">
+      <c r="G11" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="24" t="s">
+      <c r="H11" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="I11" s="24" t="s">
+      <c r="I11" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="J11" s="11"/>
-    </row>
-    <row r="12" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="46"/>
-      <c r="B12" s="53"/>
-      <c r="C12" s="55"/>
-      <c r="D12" s="51"/>
+      <c r="J11" s="9"/>
+    </row>
+    <row r="12" spans="1:10" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="50"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="56"/>
       <c r="E12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="24" t="s">
+      <c r="F12" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="G12" s="24" t="s">
+      <c r="G12" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="24" t="s">
+      <c r="H12" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="24" t="s">
+      <c r="I12" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="J12" s="11"/>
-    </row>
-    <row r="13" spans="1:10" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-    </row>
-    <row r="14" spans="1:10" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
+      <c r="J12" s="9"/>
+    </row>
+    <row r="13" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+    </row>
+    <row r="14" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="C9:C10"/>
@@ -2182,11 +2157,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:E12">
     <cfRule type="cellIs" dxfId="29" priority="1" operator="equal">
@@ -2216,336 +2186,337 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="12.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="35.44140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="22.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="50.88671875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="12.88671875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="15.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="15.0" collapsed="true"/>
-    <col min="8" max="16384" style="1" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="12.08984375" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.453125" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="50.90625" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.90625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.36328125" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="8.90625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="57" t="s">
+    <row r="1" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="38"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="57"/>
-    </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="G1" s="62"/>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="39" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:7" ht="19.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="41"/>
+      <c r="C3" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="G3" s="40"/>
+    </row>
+    <row r="4" spans="1:7" ht="19.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="C4" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="40"/>
+    </row>
+    <row r="5" spans="1:7" ht="19.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="C5" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="40"/>
+    </row>
+    <row r="6" spans="1:7" ht="19.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="40"/>
+      <c r="F6" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="40"/>
+    </row>
+    <row r="7" spans="1:7" ht="19.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="C7" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="40"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="40"/>
+    </row>
+    <row r="8" spans="1:7" ht="19.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="C8" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="40"/>
+    </row>
+    <row r="9" spans="1:7" ht="19.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="42" t="s">
+        <v>168</v>
+      </c>
+      <c r="C9" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="40"/>
+      <c r="F9" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="43" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="19.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="42" t="s">
+        <v>168</v>
+      </c>
+      <c r="C10" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="40"/>
+      <c r="F10" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" s="43" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="19.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="42" t="s">
+        <v>168</v>
+      </c>
+      <c r="C11" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="40"/>
+      <c r="F11" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" s="43" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="19.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="42" t="s">
+        <v>168</v>
+      </c>
+      <c r="C12" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="40"/>
+      <c r="F12" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" s="43" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="19.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="42" t="s">
+        <v>168</v>
+      </c>
+      <c r="C13" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="40"/>
+      <c r="F13" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="G13" s="40" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="19.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="42" t="s">
+        <v>168</v>
+      </c>
+      <c r="C14" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="40"/>
+      <c r="F14" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" s="40"/>
+    </row>
+    <row r="15" spans="1:7" ht="19.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="42" t="s">
+        <v>169</v>
+      </c>
+      <c r="C15" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="40"/>
+      <c r="F15" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="G15" s="40"/>
+    </row>
+    <row r="16" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="42"/>
+      <c r="C16" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="43" t="s">
-        <v>53</v>
-      </c>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="43" t="s">
-        <v>56</v>
-      </c>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="42" t="s">
-        <v>63</v>
-      </c>
-      <c r="G9" s="33" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="G10" s="33" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="42" t="s">
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" s="40"/>
+    </row>
+    <row r="17" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="C17" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="G11" s="33" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="42" t="s">
-        <v>74</v>
-      </c>
-      <c r="G12" s="33" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="42" t="s">
-        <v>77</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="42" t="s">
-        <v>80</v>
-      </c>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="42" t="s">
-        <v>82</v>
-      </c>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="1:7" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="1:7" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="4"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2593,9 +2564,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="F3 F9 F6 F10:F16 G9:G11" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -2607,28 +2575,28 @@
       <selection activeCell="H3" sqref="H3:H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="12.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="44.44140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="22.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="28.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="12.88671875" collapsed="true"/>
-    <col min="6" max="9" customWidth="true" style="1" width="15.33203125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="21.44140625" collapsed="true"/>
-    <col min="11" max="16384" style="1" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="12.08984375" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="44.453125" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="28.36328125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.90625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="9" width="15.36328125" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="21.453125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="16384" width="8.90625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="58" t="s">
-        <v>87</v>
-      </c>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-    </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F1" s="63" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+    </row>
+    <row r="2" spans="1:10" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2645,280 +2613,280 @@
         <v>48</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="H3" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="I3" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="J3" s="34" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+      <c r="H3" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="I3" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="J3" s="32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="33" t="s">
-        <v>103</v>
+      <c r="D4" s="31" t="s">
+        <v>88</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="H4" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="I4" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="J4" s="34"/>
-    </row>
-    <row r="5" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+      <c r="H4" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="I4" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="J4" s="32"/>
+    </row>
+    <row r="5" spans="1:10" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="H5" s="33" t="s">
-        <v>106</v>
-      </c>
-      <c r="I5" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="J5" s="34"/>
-    </row>
-    <row r="6" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="H5" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="I5" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="J5" s="32"/>
+    </row>
+    <row r="6" spans="1:10" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H6" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="H6" s="33" t="s">
-        <v>109</v>
-      </c>
-      <c r="I6" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="J6" s="34"/>
-    </row>
-    <row r="7" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I6" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="J6" s="32"/>
+    </row>
+    <row r="7" spans="1:10" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="33" t="s">
-        <v>112</v>
+      <c r="D7" s="31" t="s">
+        <v>97</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="H7" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="I7" s="33"/>
-      <c r="J7" s="34" t="s">
+      <c r="H7" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="I7" s="31"/>
+      <c r="J7" s="32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>113</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="33" t="s">
-        <v>115</v>
+      <c r="D8" s="31" t="s">
+        <v>100</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="G8" s="4"/>
-      <c r="H8" s="33" t="s">
-        <v>114</v>
-      </c>
-      <c r="I8" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="J8" s="34" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H8" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="I8" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="J8" s="32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="H9" s="4"/>
-      <c r="I9" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="J9" s="34" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I9" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="J9" s="32" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="H10" s="4"/>
-      <c r="I10" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="J10" s="34" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I10" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="J10" s="32" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="33" t="s">
-        <v>126</v>
+      <c r="D11" s="31" t="s">
+        <v>111</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="H11" s="4"/>
-      <c r="I11" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="J11" s="34" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I11" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="J11" s="32" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
     </row>
@@ -2966,30 +2934,30 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="11.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="34.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="15.5546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="23.88671875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="12.88671875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="30.88671875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="17.33203125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="9.88671875" collapsed="true"/>
-    <col min="9" max="10" customWidth="true" style="1" width="16.88671875" collapsed="true"/>
-    <col min="11" max="16384" style="1" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="11.08984375" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.54296875" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.90625" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.90625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30.90625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.36328125" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.90625" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="16.90625" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="16384" width="8.90625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="60" t="s">
+    <row r="1" spans="1:10" ht="21.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="38"/>
-    </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="34"/>
+    </row>
+    <row r="2" spans="1:10" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -3006,168 +2974,168 @@
         <v>48</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="J2" s="37" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+      <c r="J2" s="33" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="5" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="5" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="37.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="5" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="21.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="5" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J8"/>
     </row>
   </sheetData>
@@ -3212,27 +3180,27 @@
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="12.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="34.109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="22.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="28.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="12.88671875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="15.33203125" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" style="1" width="15.0" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="12.08984375" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.08984375" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="28.36328125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.90625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.36328125" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="15" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="8.90625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="62" t="s">
+    <row r="1" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="39"/>
-    </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="35"/>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -3249,136 +3217,136 @@
         <v>48</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="I2" s="40" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+      <c r="I2" s="36" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
-      <c r="I3" s="41"/>
-    </row>
-    <row r="4" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I3" s="37"/>
+    </row>
+    <row r="4" spans="1:9" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="I5" s="41" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+      <c r="I5" s="37" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="41"/>
-    </row>
-    <row r="8" spans="1:9" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="37"/>
+    </row>
+    <row r="8" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="7" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -3412,31 +3380,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0096DF0-D149-464A-950F-15761EF2F183}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="12.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="27.5546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="19.44140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="27.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="12.88671875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="22.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="15.33203125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="30.109375" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="12.08984375" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.54296875" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.453125" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="27.08984375" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.90625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.36328125" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="30.08984375" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="8.90625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="63" t="s">
+    <row r="1" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-    </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -3453,65 +3421,65 @@
         <v>48</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="27" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="25" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>190</v>
+        <v>165</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="G3" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="25" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>149</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="27" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>164</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>190</v>
+        <v>165</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>187</v>
+        <v>162</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>188</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -3557,134 +3525,139 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC5D65A6-838D-48E2-A8FC-1A09F68833D3}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="12.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="25.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="22.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="35.88671875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="12.88671875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="42.77734375" collapsed="true"/>
-    <col min="7" max="16384" style="1" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="12.08984375" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.6328125" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.54296875" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="56.08984375" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.90625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="42.81640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="8.90625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="36" t="s">
+    <row r="1" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="44"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="48" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:6" s="2" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="45" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>171</v>
+      </c>
+      <c r="C3" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="46" t="s">
+        <v>172</v>
+      </c>
+      <c r="E3" s="46"/>
+      <c r="F3" s="47" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="46" t="s">
+        <v>171</v>
+      </c>
+      <c r="C4" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="46" t="s">
+        <v>173</v>
+      </c>
+      <c r="E4" s="46"/>
+      <c r="F4" s="47" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="46" t="s">
+        <v>171</v>
+      </c>
+      <c r="C5" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="46" t="s">
+        <v>174</v>
+      </c>
+      <c r="E5" s="46"/>
+      <c r="F5" s="47" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="46" t="s">
+        <v>171</v>
+      </c>
+      <c r="C6" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="46" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="E6" s="46"/>
+      <c r="F6" s="47" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="46" t="s">
+        <v>171</v>
+      </c>
+      <c r="C7" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="34" t="s">
+      <c r="D7" s="46" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="34" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="34" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="34" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="34" t="s">
-        <v>180</v>
+      <c r="E7" s="46"/>
+      <c r="F7" s="47" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -3708,26 +3681,17 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" xr:uid="{AAE6A7E5-F198-4047-A74E-1E9BCF775FE5}"/>
-    <hyperlink ref="F4" r:id="rId2" xr:uid="{288E90AE-69C1-449D-AF3E-1BBE814413A7}"/>
-    <hyperlink ref="F5" r:id="rId3" xr:uid="{B8AEC54B-FA5A-4420-9564-0E6960CA0D3B}"/>
-    <hyperlink ref="F6" r:id="rId4" xr:uid="{A1659D58-DC14-4472-945A-B597487AA467}"/>
-    <hyperlink ref="F7" r:id="rId5" xr:uid="{A090A0E5-6A9A-405B-A6EB-1F9D2F18E84C}"/>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="F4" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="F5" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
+    <hyperlink ref="F6" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
+    <hyperlink ref="F7" r:id="rId5" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007916DAE6CBAB0E478E10A9FCA3CC0E19" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cc4eab9cdd79106b7ff0c84dd396c527">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="73b10483-4eab-47d9-97c6-997f49bd58aa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9c952eea70f5f85d64c583e57f778f77" ns2:_="">
     <xsd:import namespace="73b10483-4eab-47d9-97c6-997f49bd58aa"/>
@@ -3891,6 +3855,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -3898,14 +3871,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDA4E934-81D4-4CDA-A90D-B17985E7C5D3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF365504-DE0C-4D20-AADF-110855E1E7ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3923,6 +3888,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDA4E934-81D4-4CDA-A90D-B17985E7C5D3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D94FA3B0-7E84-4ED3-9FBD-9B6763F81478}">
   <ds:schemaRefs>

</xml_diff>